<commit_message>
Finished no combat rmd
</commit_message>
<xml_diff>
--- a/output/dmd_no_combat_planning.xlsx
+++ b/output/dmd_no_combat_planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LR\WLR\Documents-\WangLR\University\Y2S1\URECA\Code\doppelgangerSpotting\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77195AED-9C3E-44CC-98C9-30C1E0F9BA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B98CE0-F7B1-4C47-8060-96BA51ED51D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="90">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -259,16 +259,66 @@
   </si>
   <si>
     <t>Doppel_0.valid</t>
+  </si>
+  <si>
+    <t>Doppel_2.valid</t>
+  </si>
+  <si>
+    <t>Doppel_2.train</t>
+  </si>
+  <si>
+    <t>Doppel_4.train</t>
+  </si>
+  <si>
+    <t>Doppel_4.valid</t>
+  </si>
+  <si>
+    <t>Doppel_6.train</t>
+  </si>
+  <si>
+    <t>Doppel_6.valid</t>
+  </si>
+  <si>
+    <t>Doppel_8.train</t>
+  </si>
+  <si>
+    <t>Doppel_8.valid</t>
+  </si>
+  <si>
+    <t>Doppel_10.train</t>
+  </si>
+  <si>
+    <t>Doppel_10.valid</t>
+  </si>
+  <si>
+    <t>Pos_Con.train</t>
+  </si>
+  <si>
+    <t>Pos_Con.valid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,8 +344,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1704,7 +1756,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1839,165 +1891,171 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="10.90625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.75">
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2009,142 +2067,820 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FDC460C-3B4F-4B73-95B4-4E9463B1BC97}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="2" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="14" width="12.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.75">
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>